<commit_message>
update package for installation
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9511279C-5387-DA45-AE13-AB7BF611577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A08142-C9B7-644A-A161-6A856BA3C9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="1280" windowWidth="34540" windowHeight="23200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="500" windowWidth="39300" windowHeight="27080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
     <sheet name="values" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,8 +31,54 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{764FE12F-F92E-ED4D-A7A5-7B9865B27E63}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Ye;</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -583,6 +629,84 @@
   <si>
     <t>role_2</t>
   </si>
+  <si>
+    <t>name_old</t>
+  </si>
+  <si>
+    <t>grad2</t>
+  </si>
+  <si>
+    <t>gratio</t>
+  </si>
+  <si>
+    <t>winmon</t>
+  </si>
+  <si>
+    <t>seamon1</t>
+  </si>
+  <si>
+    <t>seamon2</t>
+  </si>
+  <si>
+    <t>searise</t>
+  </si>
+  <si>
+    <t>searatio</t>
+  </si>
+  <si>
+    <t>searisedays1</t>
+  </si>
+  <si>
+    <t>searisedays2</t>
+  </si>
+  <si>
+    <t>seadays</t>
+  </si>
+  <si>
+    <t>seafalldays</t>
+  </si>
+  <si>
+    <t>flooddays</t>
+  </si>
+  <si>
+    <t>frostdays</t>
+  </si>
+  <si>
+    <t>windays</t>
+  </si>
+  <si>
+    <t>floodprec</t>
+  </si>
+  <si>
+    <t>floodtemp</t>
+  </si>
+  <si>
+    <t>frosttemp</t>
+  </si>
+  <si>
+    <t>wintemp</t>
+  </si>
+  <si>
+    <t>signratio1</t>
+  </si>
+  <si>
+    <t>signratio2</t>
+  </si>
+  <si>
+    <t>gapflag</t>
+  </si>
+  <si>
+    <t>floodratio</t>
+  </si>
+  <si>
+    <t>gaplen</t>
+  </si>
+  <si>
+    <t>ismountain</t>
+  </si>
+  <si>
+    <t>Нужны ли параметры, выделенные оранжевым? Если задан режим ismountain = TRUE, нельзя ли использовать в качестве них другие параметры? Скажем, вместо polkolMount1 просто polkol1</t>
+  </si>
 </sst>
 </file>
 
@@ -591,7 +715,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,8 +774,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,8 +847,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -709,11 +874,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -759,6 +939,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -789,7 +976,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>111125</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>358775</xdr:rowOff>
@@ -1011,13 +1198,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>2931430</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1174751</xdr:rowOff>
@@ -1061,13 +1248,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>139843</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>462259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1897866</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>894456</xdr:rowOff>
@@ -1111,7 +1298,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>358775</xdr:rowOff>
@@ -1491,13 +1678,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>38947</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>527051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1620062</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>146051</xdr:rowOff>
@@ -1541,14 +1728,14 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1536703" cy="353751"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1711,10 +1898,16 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7"/>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1747,6 +1940,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="ru-RU" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1763,7 +1957,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>517525</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>333374</xdr:rowOff>
@@ -2243,63 +2437,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" customWidth="1"/>
+    <col min="10" max="10" width="129.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>106</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>111</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>112</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>113</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>114</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>115</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -2307,20 +2505,23 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
         <v>2</v>
@@ -2328,28 +2529,31 @@
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
         <v>1.5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2357,30 +2561,33 @@
       <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>6</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2388,24 +2595,27 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
         <v>150</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
     </row>
-    <row r="6" spans="1:11" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2413,23 +2623,26 @@
       <c r="B6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2437,21 +2650,24 @@
       <c r="B7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2459,18 +2675,21 @@
       <c r="B8" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2478,21 +2697,24 @@
       <c r="B9" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2500,24 +2722,27 @@
       <c r="B10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10">
         <v>30</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2525,21 +2750,24 @@
       <c r="B11" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:11" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2547,21 +2775,24 @@
       <c r="B12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2569,26 +2800,29 @@
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13">
         <v>90</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="K13" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2596,26 +2830,29 @@
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="L14" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2623,24 +2860,27 @@
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15">
         <v>15</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2648,26 +2888,29 @@
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2675,26 +2918,29 @@
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
         <v>30</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="L17" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2702,21 +2948,24 @@
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>53</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>4</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:11" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2724,21 +2973,24 @@
       <c r="B19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19">
         <v>-10</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2746,23 +2998,26 @@
       <c r="B20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20">
         <v>-1</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>61</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>60</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="K20" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2770,26 +3025,29 @@
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21">
         <v>0.01</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>68</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="L21" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2797,24 +3055,27 @@
       <c r="B22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2822,20 +3083,23 @@
       <c r="B23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23">
         <v>-999</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="K23" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2843,26 +3107,29 @@
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24">
         <v>1E-3</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2870,51 +3137,57 @@
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>27</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>74</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="K25" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>2</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="E26" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="L26" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>1000</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2922,76 +3195,82 @@
       <c r="B28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28">
         <v>0</v>
       </c>
-      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>2</v>
       </c>
-      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="21"/>
+      <c r="D30">
         <v>30</v>
       </c>
-      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="21"/>
+      <c r="D31">
         <v>5</v>
       </c>
-      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="12">
+      <c r="D32" s="12">
         <v>1.5</v>
       </c>
-      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="K26:K32"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K6:K12"/>
+    <mergeCell ref="L26:L32"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L6:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update in parameter names
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA541B86-AC2C-0549-AC23-4A9168003BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2EE064-F6E8-DE4A-9C7C-3416499DAB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="520" windowWidth="16800" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="520" windowWidth="16800" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="151">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -595,9 +595,6 @@
     <t>Mountains</t>
   </si>
   <si>
-    <t xml:space="preserve">polkolMount2 </t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>% / Vol of seasflood</t>
   </si>
   <si>
-    <t>mnt</t>
-  </si>
-  <si>
     <t>mntgrad</t>
   </si>
   <si>
@@ -740,6 +734,9 @@
   </si>
   <si>
     <t>precdays</t>
+  </si>
+  <si>
+    <t>mntmode</t>
   </si>
 </sst>
 </file>
@@ -2505,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A2" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2526,40 +2523,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>112</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -2571,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -2627,7 +2624,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2661,7 +2658,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -2689,7 +2686,7 @@
         <v>84</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2716,7 +2713,7 @@
         <v>99</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2741,7 +2738,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -2763,7 +2760,7 @@
         <v>86</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -2788,7 +2785,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -2816,7 +2813,7 @@
         <v>88</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2841,7 +2838,7 @@
         <v>89</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D12" s="20">
         <v>500</v>
@@ -2869,7 +2866,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D13">
         <v>90</v>
@@ -2899,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2929,7 +2926,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15">
         <v>15</v>
@@ -2957,7 +2954,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -2987,7 +2984,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -3017,7 +3014,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3042,7 +3039,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19">
         <v>-10</v>
@@ -3067,7 +3064,7 @@
         <v>59</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -3094,7 +3091,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" s="20">
         <v>1</v>
@@ -3103,7 +3100,7 @@
         <v>75</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>72</v>
@@ -3124,7 +3121,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>71</v>
@@ -3133,7 +3130,7 @@
         <v>76</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>72</v>
@@ -3152,7 +3149,7 @@
         <v>65</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23">
         <v>-999</v>
@@ -3176,7 +3173,7 @@
         <v>66</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="20">
         <v>0.1</v>
@@ -3185,7 +3182,7 @@
         <v>77</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>72</v>
@@ -3206,7 +3203,7 @@
         <v>67</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3233,13 +3230,13 @@
         <v>90</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" s="24" t="s">
         <v>102</v>
@@ -3270,7 +3267,7 @@
         <v>92</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -3286,7 +3283,7 @@
         <v>93</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -3295,7 +3292,7 @@
         <v>14</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L29" s="24"/>
     </row>
@@ -3308,13 +3305,13 @@
         <v>100</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D30">
         <v>30</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L30" s="24"/>
     </row>
@@ -3327,13 +3324,13 @@
         <v>101</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L31" s="24"/>
     </row>
@@ -3346,7 +3343,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D32" s="22">
         <v>150</v>
@@ -3356,7 +3353,7 @@
         <v>14</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L32" s="24"/>
     </row>
@@ -3381,8 +3378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3420,97 +3417,97 @@
         <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>21</v>
+        <v>148</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="AA1" s="12" t="s">
         <v>91</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update gaps in years
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2EE064-F6E8-DE4A-9C7C-3416499DAB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A20188-C50D-4548-BBAA-4F76533EBE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="520" windowWidth="16800" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="520" windowWidth="31060" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{764FE12F-F92E-ED4D-A7A5-7B9865B27E63}">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{764FE12F-F92E-ED4D-A7A5-7B9865B27E63}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="147">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -456,9 +456,6 @@
     <t>SignDelta1</t>
   </si>
   <si>
-    <t>FlagGaps</t>
-  </si>
-  <si>
     <t>PavRate</t>
   </si>
   <si>
@@ -471,9 +468,6 @@
     <t>значимый перепад для поиска лок.максимума</t>
   </si>
   <si>
-    <t>каким образом обозначаются пропуски в рядах</t>
-  </si>
-  <si>
     <t>SignDelta*0.15</t>
   </si>
   <si>
@@ -493,9 +487,6 @@
   </si>
   <si>
     <t xml:space="preserve">significant volume of the occasional flood in fractions of the seasonal flood volume that is considered in the analysis </t>
-  </si>
-  <si>
-    <t>The gap marker in the initial Q series</t>
   </si>
   <si>
     <r>
@@ -662,9 +653,6 @@
   </si>
   <si>
     <t>signratio2</t>
-  </si>
-  <si>
-    <t>gapflag</t>
   </si>
   <si>
     <t>floodratio</t>
@@ -2500,10 +2488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2523,40 +2511,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
-      </c>
-      <c r="J1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -2568,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -2585,7 +2573,7 @@
     </row>
     <row r="3" spans="1:12" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A31" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -2624,7 +2612,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2658,7 +2646,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -2683,10 +2671,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2710,10 +2698,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2735,10 +2723,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -2757,10 +2745,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -2782,10 +2770,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -2810,10 +2798,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2835,10 +2823,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D12" s="20">
         <v>500</v>
@@ -2866,7 +2854,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D13">
         <v>90</v>
@@ -2896,7 +2884,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2914,7 +2902,7 @@
         <v>39</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="80" x14ac:dyDescent="0.2">
@@ -2926,7 +2914,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D15">
         <v>15</v>
@@ -2954,7 +2942,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -2972,7 +2960,7 @@
         <v>46</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2984,7 +2972,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -3002,7 +2990,7 @@
         <v>50</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,7 +3002,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3039,7 +3027,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D19">
         <v>-10</v>
@@ -3064,7 +3052,7 @@
         <v>59</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -3079,7 +3067,7 @@
         <v>60</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3091,25 +3079,25 @@
         <v>63</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D21" s="20">
         <v>1</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3121,26 +3109,26 @@
         <v>64</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L22" s="25"/>
     </row>
-    <row r="23" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3149,22 +3137,28 @@
         <v>65</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23">
-        <v>-999</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>78</v>
+        <v>123</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="J23" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>82</v>
+        <v>71</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3173,88 +3167,74 @@
         <v>66</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="H24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
         <v>72</v>
       </c>
-      <c r="J24" t="s">
-        <v>73</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>83</v>
+      <c r="K24" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>67</v>
+      <c r="B25" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" t="s">
-        <v>74</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>82</v>
+      <c r="E25" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>134</v>
+        <v>88</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="L26" s="24" t="s">
-        <v>102</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="L26" s="24"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>91</v>
+      <c r="B27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="D27">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L27" s="24"/>
     </row>
@@ -3263,14 +3243,20 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>92</v>
+      <c r="B28" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="L28" s="24"/>
     </row>
@@ -3280,19 +3266,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>137</v>
+        <v>97</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L29" s="24"/>
     </row>
@@ -3302,64 +3285,45 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D30">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="22">
+        <v>150</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="L31" s="24"/>
-    </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" s="22">
-        <v>150</v>
-      </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="L32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="L26:L32"/>
+    <mergeCell ref="L25:L31"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="L17:L19"/>
     <mergeCell ref="L21:L22"/>
@@ -3376,10 +3340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3401,118 +3365,114 @@
     <col min="20" max="20" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AA1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>138</v>
-      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -3578,39 +3538,36 @@
         <v>1.5E-3</v>
       </c>
       <c r="W2">
-        <v>-999</v>
+        <v>1E-3</v>
       </c>
       <c r="X2">
-        <v>1E-3</v>
+        <v>15</v>
       </c>
       <c r="Y2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Z2">
+        <v>1000</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
         <v>2</v>
       </c>
-      <c r="AA2">
-        <v>1000</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
       <c r="AC2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="AD2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="AE2">
-        <v>5</v>
-      </c>
-      <c r="AF2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -3676,39 +3633,36 @@
         <v>2.2499999999999998E-3</v>
       </c>
       <c r="W3">
-        <v>-999</v>
+        <v>2E-3</v>
       </c>
       <c r="X3">
-        <v>2E-3</v>
+        <v>13</v>
       </c>
       <c r="Y3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="Z3">
-        <v>2</v>
+        <v>900</v>
       </c>
       <c r="AA3">
-        <v>900</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AC3">
+        <v>20</v>
+      </c>
+      <c r="AD3">
         <v>4</v>
       </c>
-      <c r="AD3">
-        <v>20</v>
-      </c>
       <c r="AE3">
-        <v>4</v>
-      </c>
-      <c r="AF3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -3774,33 +3728,30 @@
         <v>1.5E-3</v>
       </c>
       <c r="W4">
-        <v>-999</v>
+        <v>2E-3</v>
       </c>
       <c r="X4">
-        <v>2E-3</v>
+        <v>14</v>
       </c>
       <c r="Y4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="Z4">
-        <v>2</v>
+        <v>950</v>
       </c>
       <c r="AA4">
-        <v>950</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="AD4">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="AE4">
-        <v>4</v>
-      </c>
-      <c r="AF4">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update package with frechet decay
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49444AA0-DD27-034B-AEA8-32D05A26C760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AA3569-8D1E-1245-A00E-6B902DEF81EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16660" yWindow="5240" windowWidth="31060" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12900" yWindow="500" windowWidth="31060" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="155">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -725,6 +725,30 @@
   </si>
   <si>
     <t>mntmode</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>padding</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aq</t>
+  </si>
+  <si>
+    <t>passes</t>
+  </si>
+  <si>
+    <t>lynehollick</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>niter</t>
   </si>
 </sst>
 </file>
@@ -2490,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A12" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3340,10 +3364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3374,7 +3398,7 @@
     <col min="31" max="31" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>95</v>
       </c>
@@ -3468,8 +3492,32 @@
       <c r="AE1" s="12" t="s">
         <v>134</v>
       </c>
+      <c r="AF1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -3563,8 +3611,32 @@
       <c r="AE2">
         <v>1.5</v>
       </c>
+      <c r="AF2">
+        <v>100</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH2">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AI2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AJ2">
+        <v>0.05</v>
+      </c>
+      <c r="AK2">
+        <v>-0.5</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -3658,8 +3730,32 @@
       <c r="AE3">
         <v>2.5</v>
       </c>
+      <c r="AF3">
+        <v>100</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH3">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AI3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AJ3">
+        <v>0.05</v>
+      </c>
+      <c r="AK3">
+        <v>-0.5</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -3752,6 +3848,30 @@
       </c>
       <c r="AE4">
         <v>2.5</v>
+      </c>
+      <c r="AF4">
+        <v>100</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH4">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AI4">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AJ4">
+        <v>0.05</v>
+      </c>
+      <c r="AK4">
+        <v>-0.5</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tests to params
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93187F75-81E8-8A41-B514-073FE0F2C6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4BBE7C-6E64-3446-B1DE-DF82070B005E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="500" windowWidth="31060" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{764FE12F-F92E-ED4D-A7A5-7B9865B27E63}">
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{764FE12F-F92E-ED4D-A7A5-7B9865B27E63}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>интенсивность спада/подъема расхода воды за счет грунтовой составляющей, выраженная в долях от расхода предшествующего дня</t>
-  </si>
-  <si>
-    <t>%/day</t>
   </si>
   <si>
     <t>rate of durial change in discharge of ground-routed waters</t>
@@ -407,9 +404,6 @@
     <t>средняя суточная температура не более Twin к ряду nWin дней для перехода к зимнему сезону</t>
   </si>
   <si>
-    <t>С</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Summer switches on winter after </t>
     </r>
@@ -468,9 +462,6 @@
     <t>значимый перепад для поиска лок.максимума</t>
   </si>
   <si>
-    <t>SignDelta*0.15</t>
-  </si>
-  <si>
     <t>doesn't have a strick physical meaning</t>
   </si>
   <si>
@@ -586,9 +577,6 @@
     <t>Mountains</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -661,9 +649,6 @@
     <t>gaplen</t>
   </si>
   <si>
-    <t>Нужны ли параметры, выделенные оранжевым? Если задан режим ismountain = TRUE, нельзя ли использовать в качестве них другие параметры? Скажем, вместо polkolMount1 просто polkol1</t>
-  </si>
-  <si>
     <t>Во сколько раз средний расход воды за каждые последовательно polkolMount(1) дней в течение общего периода polkolMount(2) превышают предшествующий половодью меженный уровень</t>
   </si>
   <si>
@@ -679,12 +664,6 @@
     <t>snowtemp</t>
   </si>
   <si>
-    <t>% / Qmax</t>
-  </si>
-  <si>
-    <t>% / Vol of seasflood</t>
-  </si>
-  <si>
     <t>mntgrad</t>
   </si>
   <si>
@@ -752,6 +731,90 @@
   </si>
   <si>
     <t>ftcomp</t>
+  </si>
+  <si>
+    <t>spcomp</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>how much longer should be the spring flood than sprecdays to activate the exponential recession curve</t>
+  </si>
+  <si>
+    <t>Celsius degrees</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>m3s/day</t>
+  </si>
+  <si>
+    <t>lowest temperature for rain flood. If lower, then the flood is considered a thaw</t>
+  </si>
+  <si>
+    <t>lowest temperature for snow event</t>
+  </si>
+  <si>
+    <t>the absolute gradient of the flow that can be considered the end of the spring flood event</t>
+  </si>
+  <si>
+    <t>Enable mountain mode. Separation is made using different approach then.</t>
+  </si>
+  <si>
+    <t>Critical gradient of change in daily discharge characteristic of the "base wave" of seasonal flooding in mountain rivers, formed by melting snow and ice in the basin, expressed as a fraction of the previous day's discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow averaging window to test the 3rd criterion for the onset of flooding in the mountainous regime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The period of time during which the average water discharge for each mntavgdays day exceeds the preceding flood level by at least a polgradMount of times </t>
+  </si>
+  <si>
+    <t>How many times the average flow rate for each successive mntavgdays days during the total period mntratiodays exceeds the preceding flood level</t>
+  </si>
+  <si>
+    <t>A number of iterations used to jitter separation parameters if spring flood cannot be identified with default values</t>
+  </si>
+  <si>
+    <t>Baseflow filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric value of a filtering parameter used in 'chapman', 'jakeman' and 'lynehollick' methods. </t>
+  </si>
+  <si>
+    <t>Numeric value of a separation shape parameter used in 'boughton', 'jakeman' and 'maxwell' methods</t>
+  </si>
+  <si>
+    <t>Numeric value of a filtering parameter used in 'jakeman' method</t>
+  </si>
+  <si>
+    <t>Numeric value of a filtering parameter used in 'boughton' and 'maxwell' methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer number of elements padded at the beginning and ending of runoff vector to reduce boundary effects. </t>
+  </si>
+  <si>
+    <t>Integer number of filtering iterations. The first iteration is forward, second is backward, third is forward and so on</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -761,7 +824,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -806,15 +869,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -834,14 +888,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -864,8 +910,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Основной текст)"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,19 +980,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,18 +998,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -965,26 +1011,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1013,22 +1044,14 @@
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1044,11 +1067,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1359,8 +1395,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1877009</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1507253</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>86274</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1788,9 +1824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1306129</xdr:colOff>
+      <xdr:colOff>657807</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>146051</xdr:rowOff>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1831,14 +1867,14 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>623144</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>69894</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1536703" cy="353751"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1852,7 +1888,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4876800" y="7943850"/>
+              <a:off x="6502445" y="10789404"/>
               <a:ext cx="1536703" cy="353751"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2001,7 +2037,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2015,7 +2051,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4876800" y="7943850"/>
+              <a:off x="6502445" y="10789404"/>
               <a:ext cx="1536703" cy="353751"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2060,14 +2096,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>517525</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>801721</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>333374</xdr:rowOff>
+      <xdr:rowOff>306731</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="993775" cy="365806"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -2081,7 +2117,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5197475" y="8715374"/>
+              <a:off x="6681022" y="11567990"/>
               <a:ext cx="993775" cy="365806"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2207,15 +2243,21 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="TextBox 9"/>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5197475" y="8715374"/>
+              <a:off x="6681022" y="11567990"/>
               <a:ext cx="993775" cy="365806"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2243,6 +2285,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="ru-RU" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2253,13 +2296,13 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑘𝑜𝑙(3)</a:t>
+                <a:t>𝑘𝑜𝑙(3))</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>))/</a:t>
+                <a:t>)/</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="ru-RU" sz="1100" i="0">
@@ -2541,22 +2584,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="188.1640625" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" customWidth="1"/>
     <col min="12" max="12" width="8.1640625" customWidth="1"/>
@@ -2564,40 +2608,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -2605,11 +2649,11 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>114</v>
+      <c r="C2" s="30" t="s">
+        <v>110</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -2617,6 +2661,9 @@
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
@@ -2626,33 +2673,33 @@
     </row>
     <row r="3" spans="1:12" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A31" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A40" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>8</v>
+      <c r="C3" s="32" t="s">
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1.5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="26" t="s">
-        <v>18</v>
+      <c r="K3" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="L3" s="6"/>
     </row>
@@ -2661,88 +2708,91 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>112</v>
+      <c r="B4" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="H4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="288" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="L4" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>113</v>
+      <c r="B5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>109</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="27"/>
+        <v>11</v>
+      </c>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>137</v>
+      <c r="B6" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>130</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>151</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -2750,636 +2800,867 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>138</v>
+      <c r="B7" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>151</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="28"/>
-    </row>
-    <row r="8" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>139</v>
+      <c r="B8" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>132</v>
       </c>
       <c r="D8">
         <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="28"/>
+        <v>16</v>
+      </c>
+      <c r="L8" s="24"/>
     </row>
     <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>140</v>
+      <c r="B9" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>133</v>
       </c>
       <c r="D9">
         <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="28"/>
+        <v>22</v>
+      </c>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>141</v>
+      <c r="B10" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>134</v>
       </c>
       <c r="D10">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="28"/>
+        <v>23</v>
+      </c>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>142</v>
+      <c r="B11" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="28"/>
+        <v>27</v>
+      </c>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" s="20">
-        <v>500</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>14</v>
+      <c r="B12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="28">
+        <v>6</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>144</v>
+      <c r="B13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>137</v>
       </c>
       <c r="D13">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>145</v>
+      <c r="B14" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>149</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>115</v>
+      <c r="B15" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>138</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" t="s">
         <v>38</v>
       </c>
-      <c r="J15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" ht="124" x14ac:dyDescent="0.2">
+      <c r="L15" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="J16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="L16" s="21"/>
+    </row>
+    <row r="17" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>117</v>
+      <c r="B17" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="J17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>119</v>
+      <c r="B19" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="D19">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>154</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="25"/>
-    </row>
-    <row r="20" spans="1:12" ht="124" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="L19" s="21"/>
+    </row>
+    <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>120</v>
+      <c r="B20" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>115</v>
       </c>
       <c r="D20">
-        <v>-1</v>
+        <v>-10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="J20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="20">
-        <v>1</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>70</v>
+      <c r="B21" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>154</v>
       </c>
       <c r="J21" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="128" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="B22" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" t="s">
-        <v>68</v>
-      </c>
-      <c r="L22" s="25"/>
-    </row>
-    <row r="23" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>132</v>
+      <c r="B23" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="28">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J23" t="s">
-        <v>71</v>
-      </c>
-      <c r="L23" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" t="s">
-        <v>27</v>
+      <c r="B24" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="J24" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>130</v>
+      <c r="B25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>120</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>88</v>
+      <c r="B26" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="D26">
-        <v>1000</v>
-      </c>
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" t="s">
+        <v>154</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>146</v>
+      <c r="B27" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="L27" s="24"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="L27" s="20"/>
+    </row>
+    <row r="28" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>133</v>
+      <c r="B28" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>139</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="L28" s="24"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="L28" s="20"/>
+    </row>
+    <row r="29" spans="1:12" ht="128" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>135</v>
+      <c r="B29" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="D29">
-        <v>30</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="L29" s="24"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="L29" s="20"/>
+    </row>
+    <row r="30" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>136</v>
+      <c r="B30" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>128</v>
       </c>
       <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="L30" s="24"/>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="L30" s="20"/>
+    </row>
+    <row r="31" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="22">
+      <c r="B31" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="34">
         <v>150</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="L31" s="24"/>
+      <c r="E32" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="L32" s="20"/>
+    </row>
+    <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>0.05</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38">
+        <v>-0.5</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39">
+        <v>30</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F40" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="L25:L31"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="L26:L32"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="L22:L23"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="L6:L12"/>
@@ -3395,8 +3676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AF28" sqref="AF28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3429,130 +3710,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="T1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="AC1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="AK1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="AN1" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="AE1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG1" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH1" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="AI1" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ1" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK1" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL1" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM1" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN1" s="30" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -3590,7 +3871,7 @@
       <c r="M2">
         <v>20</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="19">
         <v>2</v>
       </c>
       <c r="O2">
@@ -3647,34 +3928,34 @@
       <c r="AF2">
         <v>1.5</v>
       </c>
-      <c r="AG2" s="31">
+      <c r="AG2" s="17">
         <v>100</v>
       </c>
-      <c r="AH2" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI2" s="31">
+      <c r="AH2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI2" s="17">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AJ2" s="31">
+      <c r="AJ2" s="17">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AK2" s="31">
+      <c r="AK2" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL2" s="31">
+      <c r="AL2" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM2" s="31">
+      <c r="AM2" s="17">
         <v>0</v>
       </c>
-      <c r="AN2" s="31">
+      <c r="AN2" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -3712,7 +3993,7 @@
       <c r="M3">
         <v>20</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="19">
         <v>2</v>
       </c>
       <c r="O3">
@@ -3769,34 +4050,34 @@
       <c r="AF3">
         <v>2.5</v>
       </c>
-      <c r="AG3" s="31">
+      <c r="AG3" s="17">
         <v>100</v>
       </c>
-      <c r="AH3" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI3" s="31">
+      <c r="AH3" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI3" s="17">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AJ3" s="31">
+      <c r="AJ3" s="17">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AK3" s="31">
+      <c r="AK3" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL3" s="31">
+      <c r="AL3" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM3" s="31">
+      <c r="AM3" s="17">
         <v>0</v>
       </c>
-      <c r="AN3" s="31">
+      <c r="AN3" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -3834,7 +4115,7 @@
       <c r="M4">
         <v>20</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="19">
         <v>2</v>
       </c>
       <c r="O4">
@@ -3891,36 +4172,36 @@
       <c r="AF4">
         <v>2.5</v>
       </c>
-      <c r="AG4" s="31">
+      <c r="AG4" s="17">
         <v>100</v>
       </c>
-      <c r="AH4" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI4" s="31">
+      <c r="AH4" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI4" s="17">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AJ4" s="31">
+      <c r="AJ4" s="17">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AK4" s="31">
+      <c r="AK4" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL4" s="31">
+      <c r="AL4" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM4" s="31">
+      <c r="AM4" s="17">
         <v>0</v>
       </c>
-      <c r="AN4" s="31">
+      <c r="AN4" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="N5" s="29"/>
+      <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="N6" s="29"/>
+      <c r="N6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename english plot titles
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4BBE7C-6E64-3446-B1DE-DF82070B005E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419871EB-1CD1-1B4B-96FD-0119F31CADC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,21 +1053,6 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1084,6 +1069,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1873,8 +1873,8 @@
       <xdr:rowOff>69894</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1536703" cy="353751"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2037,7 +2037,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2102,8 +2102,8 @@
       <xdr:rowOff>306731</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="993775" cy="365806"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -2243,7 +2243,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -2586,15 +2586,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -2613,7 +2613,7 @@
       <c r="B1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D1" t="s">
@@ -2649,10 +2649,10 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="25" t="s">
         <v>110</v>
       </c>
       <c r="D2">
@@ -2676,10 +2676,10 @@
         <f t="shared" ref="A3:A40" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D3">
@@ -2698,7 +2698,7 @@
       <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="34" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="6"/>
@@ -2708,10 +2708,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="27" t="s">
         <v>108</v>
       </c>
       <c r="D4">
@@ -2732,8 +2732,8 @@
       <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23" t="s">
+      <c r="K4" s="34"/>
+      <c r="L4" s="35" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2742,10 +2742,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>109</v>
       </c>
       <c r="D5">
@@ -2763,17 +2763,17 @@
       <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="23"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>130</v>
       </c>
       <c r="D6">
@@ -2791,7 +2791,7 @@
       <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="36" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2800,10 +2800,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="25" t="s">
         <v>131</v>
       </c>
       <c r="D7">
@@ -2821,17 +2821,17 @@
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="24"/>
+      <c r="L7" s="36"/>
     </row>
     <row r="8" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="27" t="s">
         <v>132</v>
       </c>
       <c r="D8">
@@ -2846,17 +2846,17 @@
       <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="24"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="27" t="s">
         <v>133</v>
       </c>
       <c r="D9">
@@ -2871,17 +2871,17 @@
       <c r="J9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="24"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="27" t="s">
         <v>134</v>
       </c>
       <c r="D10">
@@ -2899,17 +2899,17 @@
       <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="24"/>
+      <c r="L10" s="36"/>
     </row>
     <row r="11" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="27" t="s">
         <v>135</v>
       </c>
       <c r="D11">
@@ -2924,23 +2924,23 @@
       <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="24"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="1:12" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="23">
         <v>6</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="30" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -2952,17 +2952,17 @@
       <c r="J12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="24"/>
+      <c r="L12" s="36"/>
     </row>
     <row r="13" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>137</v>
       </c>
       <c r="D13">
@@ -2988,10 +2988,10 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="25" t="s">
         <v>149</v>
       </c>
       <c r="D14">
@@ -3011,10 +3011,10 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="25" t="s">
         <v>138</v>
       </c>
       <c r="D15">
@@ -3032,7 +3032,7 @@
       <c r="J15" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="33" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3041,10 +3041,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="25" t="s">
         <v>111</v>
       </c>
       <c r="D16">
@@ -3062,17 +3062,17 @@
       <c r="J16" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="21"/>
+      <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="25" t="s">
         <v>112</v>
       </c>
       <c r="D17">
@@ -3099,10 +3099,10 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="25" t="s">
         <v>113</v>
       </c>
       <c r="D18">
@@ -3120,7 +3120,7 @@
       <c r="J18" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="21" t="s">
+      <c r="L18" s="33" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3129,10 +3129,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="25" t="s">
         <v>114</v>
       </c>
       <c r="D19">
@@ -3150,17 +3150,17 @@
       <c r="J19" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="21"/>
+      <c r="L19" s="33"/>
     </row>
     <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="27" t="s">
         <v>115</v>
       </c>
       <c r="D20">
@@ -3175,17 +3175,17 @@
       <c r="J20" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="21"/>
+      <c r="L20" s="33"/>
     </row>
     <row r="21" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="27" t="s">
         <v>116</v>
       </c>
       <c r="D21">
@@ -3209,16 +3209,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="23">
         <v>0.01</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="30" t="s">
         <v>70</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -3230,7 +3230,7 @@
       <c r="J22" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="21" t="s">
+      <c r="L22" s="33" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3239,16 +3239,16 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="23">
         <v>1.5E-3</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="30" t="s">
         <v>71</v>
       </c>
       <c r="F23" s="14" t="s">
@@ -3260,23 +3260,23 @@
       <c r="J23" t="s">
         <v>66</v>
       </c>
-      <c r="L23" s="21"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="23">
         <v>0.1</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="30" t="s">
         <v>72</v>
       </c>
       <c r="F24" s="14" t="s">
@@ -3297,10 +3297,10 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="25" t="s">
         <v>120</v>
       </c>
       <c r="D25">
@@ -3324,22 +3324,22 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="27" t="s">
         <v>125</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="31" t="s">
         <v>161</v>
       </c>
       <c r="F26" t="s">
         <v>154</v>
       </c>
-      <c r="L26" s="20" t="s">
+      <c r="L26" s="32" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3348,10 +3348,10 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="27" t="s">
         <v>85</v>
       </c>
       <c r="D27">
@@ -3360,20 +3360,20 @@
       <c r="E27" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="L27" s="20"/>
+      <c r="L27" s="32"/>
     </row>
     <row r="28" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="27" t="s">
         <v>139</v>
       </c>
       <c r="D28">
@@ -3385,17 +3385,17 @@
       <c r="F28" t="s">
         <v>158</v>
       </c>
-      <c r="L28" s="20"/>
+      <c r="L28" s="32"/>
     </row>
     <row r="29" spans="1:12" ht="128" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="27" t="s">
         <v>126</v>
       </c>
       <c r="D29">
@@ -3410,17 +3410,17 @@
       <c r="J29" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="L29" s="20"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="27" t="s">
         <v>128</v>
       </c>
       <c r="D30">
@@ -3435,17 +3435,17 @@
       <c r="J30" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="L30" s="20"/>
+      <c r="L30" s="32"/>
     </row>
     <row r="31" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="27" t="s">
         <v>129</v>
       </c>
       <c r="D31">
@@ -3460,23 +3460,23 @@
       <c r="J31" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="L31" s="20"/>
+      <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="29">
         <v>150</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="30" t="s">
         <v>167</v>
       </c>
       <c r="F32" s="14" t="s">
@@ -3485,17 +3485,17 @@
       <c r="J32" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="L32" s="20"/>
+      <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="25" t="s">
         <v>147</v>
       </c>
       <c r="D33">
@@ -3513,13 +3513,13 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="20" t="s">
         <v>145</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -3534,10 +3534,10 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="25" t="s">
         <v>142</v>
       </c>
       <c r="D35">
@@ -3555,10 +3555,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="25" t="s">
         <v>140</v>
       </c>
       <c r="D36">
@@ -3576,10 +3576,10 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="25" t="s">
         <v>52</v>
       </c>
       <c r="D37">
@@ -3597,10 +3597,10 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="25" t="s">
         <v>143</v>
       </c>
       <c r="D38">
@@ -3618,10 +3618,10 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="25" t="s">
         <v>141</v>
       </c>
       <c r="D39">
@@ -3639,10 +3639,10 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="25" t="s">
         <v>144</v>
       </c>
       <c r="D40">

</xml_diff>

<commit_message>
add spatial regions and rename spring params
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419871EB-1CD1-1B4B-96FD-0119F31CADC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAE873E-BCB1-C646-8FCD-F0BCA32E059B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6340" yWindow="500" windowWidth="26000" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="183">
   <si>
     <t>месяц, с которого начинается зимняя межень</t>
   </si>
@@ -553,15 +553,6 @@
     <t xml:space="preserve">polgradMount </t>
   </si>
   <si>
-    <t>Caucasus</t>
-  </si>
-  <si>
-    <t>Urals</t>
-  </si>
-  <si>
-    <t>Midplain</t>
-  </si>
-  <si>
     <t>region</t>
   </si>
   <si>
@@ -676,30 +667,6 @@
     <t>mntratiodays</t>
   </si>
   <si>
-    <t>ftmon1</t>
-  </si>
-  <si>
-    <t>ftmon2</t>
-  </si>
-  <si>
-    <t>ftrisedays1</t>
-  </si>
-  <si>
-    <t>ftrisedays2</t>
-  </si>
-  <si>
-    <t>ftdays</t>
-  </si>
-  <si>
-    <t>ftrise</t>
-  </si>
-  <si>
-    <t>ftratio</t>
-  </si>
-  <si>
-    <t>ftrecdays</t>
-  </si>
-  <si>
     <t>precdays</t>
   </si>
   <si>
@@ -730,9 +697,6 @@
     <t>niter</t>
   </si>
   <si>
-    <t>ftcomp</t>
-  </si>
-  <si>
     <t>spcomp</t>
   </si>
   <si>
@@ -815,6 +779,60 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>gradabs</t>
+  </si>
+  <si>
+    <t>northwest</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>northeast</t>
+  </si>
+  <si>
+    <t>volga</t>
+  </si>
+  <si>
+    <t>oka</t>
+  </si>
+  <si>
+    <t>southeast</t>
+  </si>
+  <si>
+    <t>spmon1</t>
+  </si>
+  <si>
+    <t>spmon2</t>
+  </si>
+  <si>
+    <t>sprisedays1</t>
+  </si>
+  <si>
+    <t>sprisedays2</t>
+  </si>
+  <si>
+    <t>spdays</t>
+  </si>
+  <si>
+    <t>sprise</t>
+  </si>
+  <si>
+    <t>spratio</t>
+  </si>
+  <si>
+    <t>sprecdays</t>
+  </si>
+  <si>
+    <t>sptrisedays1</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -824,7 +842,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -896,21 +914,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -928,8 +931,16 @@
       <name val="Calibri (Основной текст)"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,12 +991,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -994,12 +999,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1015,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1043,31 +1042,25 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1085,6 +1078,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2586,15 +2581,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -2608,40 +2603,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -2649,11 +2644,11 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>110</v>
+      <c r="C2" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -2662,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2676,10 +2671,10 @@
         <f t="shared" ref="A3:A40" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D3">
@@ -2689,7 +2684,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
@@ -2698,7 +2693,7 @@
       <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="6"/>
@@ -2708,11 +2703,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>108</v>
+      <c r="C4" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2721,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>9</v>
@@ -2732,8 +2727,8 @@
       <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2742,11 +2737,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>109</v>
+      <c r="C5" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -2763,18 +2758,18 @@
       <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="35"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>130</v>
+      <c r="C6" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2783,7 +2778,7 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>25</v>
@@ -2791,7 +2786,7 @@
       <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="L6" s="30" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2800,11 +2795,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>131</v>
+      <c r="B7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>174</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2813,7 +2808,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>25</v>
@@ -2821,18 +2816,18 @@
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>132</v>
+      <c r="C8" s="21" t="s">
+        <v>181</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -2846,18 +2841,18 @@
       <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="36"/>
+      <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>133</v>
+      <c r="C9" s="21" t="s">
+        <v>176</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -2871,18 +2866,18 @@
       <c r="J9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="36"/>
+      <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>134</v>
+      <c r="C10" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -2899,18 +2894,18 @@
       <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="36"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>135</v>
+      <c r="C11" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2924,27 +2919,27 @@
       <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="36"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="23">
+      <c r="C12" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="17">
         <v>6</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>152</v>
+      <c r="F12" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>25</v>
@@ -2952,18 +2947,18 @@
       <c r="J12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="36"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>137</v>
+      <c r="C13" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="D13">
         <v>20</v>
@@ -2988,20 +2983,20 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>149</v>
+      <c r="B14" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>137</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H14" s="3"/>
       <c r="K14" s="7"/>
@@ -3011,11 +3006,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>138</v>
+      <c r="C15" s="19" t="s">
+        <v>127</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -3032,7 +3027,7 @@
       <c r="J15" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3041,11 +3036,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>111</v>
+      <c r="C16" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -3062,18 +3057,18 @@
       <c r="J16" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="33"/>
+      <c r="L16" s="27"/>
     </row>
     <row r="17" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>112</v>
+      <c r="C17" s="19" t="s">
+        <v>109</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -3099,11 +3094,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>113</v>
+      <c r="C18" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="D18">
         <v>30</v>
@@ -3120,7 +3115,7 @@
       <c r="J18" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3129,20 +3124,20 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>114</v>
+      <c r="C19" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F19" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="H19" t="s">
         <v>4</v>
@@ -3150,18 +3145,18 @@
       <c r="J19" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="33"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>115</v>
+      <c r="C20" s="21" t="s">
+        <v>112</v>
       </c>
       <c r="D20">
         <v>-10</v>
@@ -3170,23 +3165,23 @@
         <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="J20" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="33"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="1:12" ht="124" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>116</v>
+      <c r="C21" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -3195,7 +3190,7 @@
         <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="J21" t="s">
         <v>59</v>
@@ -3209,20 +3204,20 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="23">
+      <c r="C22" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="17">
         <v>0.01</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>152</v>
+      <c r="F22" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>67</v>
@@ -3230,7 +3225,7 @@
       <c r="J22" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="33" t="s">
+      <c r="L22" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3239,20 +3234,20 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="23">
+      <c r="C23" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="17">
         <v>1.5E-3</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>152</v>
+      <c r="F23" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>67</v>
@@ -3260,27 +3255,27 @@
       <c r="J23" t="s">
         <v>66</v>
       </c>
-      <c r="L23" s="33"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="23">
+      <c r="C24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="17">
         <v>0.1</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>152</v>
+      <c r="F24" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>67</v>
@@ -3297,11 +3292,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>120</v>
+      <c r="C25" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3324,23 +3319,23 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>125</v>
+      <c r="C26" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>161</v>
+      <c r="E26" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="F26" t="s">
-        <v>154</v>
-      </c>
-      <c r="L26" s="32" t="s">
-        <v>96</v>
+        <v>142</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -3348,164 +3343,164 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="21" t="s">
         <v>85</v>
       </c>
       <c r="D27">
         <v>1000</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="L27" s="32"/>
+        <v>150</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>139</v>
+      <c r="C28" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
-      </c>
-      <c r="L28" s="32"/>
+        <v>146</v>
+      </c>
+      <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" ht="128" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="27" t="s">
-        <v>126</v>
+      <c r="C29" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="L29" s="32"/>
+      <c r="J29" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L29" s="26"/>
     </row>
     <row r="30" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>128</v>
+      <c r="B30" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D30">
         <v>30</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F30" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="L30" s="32"/>
+      <c r="J30" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>129</v>
+      <c r="B31" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="L31" s="32"/>
+      <c r="J31" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L31" s="26"/>
     </row>
     <row r="32" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="29">
+      <c r="C32" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="23">
         <v>150</v>
       </c>
-      <c r="E32" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="L32" s="32"/>
+      <c r="J32" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="L32" s="26"/>
     </row>
     <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>147</v>
+      <c r="B33" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="D33">
         <v>100</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3513,20 +3508,20 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>145</v>
+      <c r="B34" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3534,20 +3529,20 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>142</v>
+      <c r="B35" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="D35">
         <v>0.92500000000000004</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -3555,20 +3550,20 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>140</v>
+      <c r="B36" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>129</v>
       </c>
       <c r="D36">
         <v>0.97499999999999998</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3576,20 +3571,20 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="25" t="s">
+      <c r="B37" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D37">
         <v>0.05</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -3597,20 +3592,20 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>143</v>
+      <c r="B38" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D38">
         <v>-0.5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F38" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3618,17 +3613,17 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>141</v>
+      <c r="B39" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="D39">
         <v>30</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F39" t="s">
         <v>26</v>
@@ -3639,20 +3634,20 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>144</v>
+      <c r="B40" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F40" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3674,205 +3669,181 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" customWidth="1"/>
-    <col min="15" max="15" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="T1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U1" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" t="s">
+        <v>114</v>
+      </c>
+      <c r="X1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH1" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI1" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK1" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM1" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN1" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO1" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>3.5</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>800</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y1" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1.5</v>
-      </c>
-      <c r="E2">
-        <v>1500</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>15</v>
-      </c>
       <c r="J2">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <v>10</v>
       </c>
       <c r="L2">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="M2">
-        <v>20</v>
-      </c>
-      <c r="N2" s="19">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>25</v>
       </c>
       <c r="O2">
         <v>2</v>
@@ -3884,117 +3855,120 @@
         <v>5</v>
       </c>
       <c r="R2">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
         <v>0</v>
       </c>
-      <c r="T2">
-        <v>-5</v>
-      </c>
       <c r="U2">
+        <v>-8</v>
+      </c>
+      <c r="V2">
         <v>-1</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>0.01</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>1.5E-3</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>1E-3</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>15</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>2</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>1000</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>2</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>30</v>
       </c>
-      <c r="AE2">
-        <v>5</v>
-      </c>
       <c r="AF2">
+        <v>5</v>
+      </c>
+      <c r="AG2">
         <v>1.5</v>
       </c>
-      <c r="AG2" s="17">
+      <c r="AH2" s="17">
         <v>100</v>
       </c>
-      <c r="AH2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI2" s="17">
-        <v>0.92500000000000004</v>
+      <c r="AI2" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="AJ2" s="17">
-        <v>0.97499999999999998</v>
+        <v>0.93</v>
       </c>
       <c r="AK2" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL2" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL2" s="17">
+      <c r="AM2" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM2" s="17">
+      <c r="AN2" s="17">
         <v>0</v>
       </c>
-      <c r="AN2" s="17">
+      <c r="AO2" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1.7</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1200</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>25</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
         <v>30</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
       <c r="M3">
-        <v>20</v>
-      </c>
-      <c r="N3" s="19">
-        <v>2</v>
+        <v>2.5</v>
+      </c>
+      <c r="N3">
+        <v>35</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -4006,202 +3980,702 @@
         <v>5</v>
       </c>
       <c r="R3">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
         <v>0</v>
       </c>
-      <c r="T3">
-        <v>-5</v>
-      </c>
       <c r="U3">
+        <v>-8</v>
+      </c>
+      <c r="V3">
         <v>-1</v>
       </c>
-      <c r="V3">
-        <v>1.4999999999999999E-2</v>
-      </c>
       <c r="W3">
-        <v>2.2499999999999998E-3</v>
+        <v>0.01</v>
       </c>
       <c r="X3">
-        <v>2E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="Y3">
-        <v>13</v>
+        <v>1E-3</v>
       </c>
       <c r="Z3">
+        <v>15</v>
+      </c>
+      <c r="AA3">
         <v>2</v>
       </c>
-      <c r="AA3">
-        <v>900</v>
-      </c>
       <c r="AB3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="AC3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="AE3">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="AF3">
-        <v>2.5</v>
-      </c>
-      <c r="AG3" s="17">
+        <v>5</v>
+      </c>
+      <c r="AG3">
+        <v>1.5</v>
+      </c>
+      <c r="AH3" s="17">
         <v>100</v>
       </c>
-      <c r="AH3" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI3" s="17">
+      <c r="AI3" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ3" s="17">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AJ3" s="17">
-        <v>0.97499999999999998</v>
-      </c>
       <c r="AK3" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL3" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL3" s="17">
+      <c r="AM3" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM3" s="17">
+      <c r="AN3" s="17">
         <v>0</v>
       </c>
-      <c r="AN3" s="17">
+      <c r="AO3" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1100</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K4">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="M4">
-        <v>20</v>
-      </c>
-      <c r="N4" s="19">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>60</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>-8</v>
+      </c>
+      <c r="V4">
+        <v>-1</v>
+      </c>
+      <c r="W4">
+        <v>0.01</v>
+      </c>
+      <c r="X4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="Y4">
+        <v>1E-3</v>
+      </c>
+      <c r="Z4">
+        <v>15</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>1000</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4">
+        <v>30</v>
+      </c>
+      <c r="AF4">
+        <v>5</v>
+      </c>
+      <c r="AG4">
+        <v>1.5</v>
+      </c>
+      <c r="AH4" s="17">
+        <v>100</v>
+      </c>
+      <c r="AI4" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ4" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AK4" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL4" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="AM4" s="17">
+        <v>-0.5</v>
+      </c>
+      <c r="AN4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="Q4">
-        <v>5</v>
-      </c>
-      <c r="R4">
-        <v>0.2</v>
-      </c>
-      <c r="S4">
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
         <v>0</v>
       </c>
-      <c r="T4">
-        <v>-4</v>
-      </c>
-      <c r="U4">
+      <c r="U5">
+        <v>-8</v>
+      </c>
+      <c r="V5">
         <v>-1</v>
       </c>
-      <c r="V4">
+      <c r="W5">
         <v>0.01</v>
       </c>
-      <c r="W4">
+      <c r="X5">
         <v>1.5E-3</v>
       </c>
-      <c r="X4">
-        <v>2E-3</v>
-      </c>
-      <c r="Y4">
-        <v>14</v>
-      </c>
-      <c r="Z4">
+      <c r="Y5">
+        <v>1E-3</v>
+      </c>
+      <c r="Z5">
+        <v>15</v>
+      </c>
+      <c r="AA5">
         <v>2</v>
       </c>
-      <c r="AA4">
-        <v>950</v>
-      </c>
-      <c r="AB4">
-        <v>1</v>
-      </c>
-      <c r="AC4">
+      <c r="AB5">
+        <v>1000</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>2</v>
+      </c>
+      <c r="AE5">
+        <v>30</v>
+      </c>
+      <c r="AF5">
+        <v>5</v>
+      </c>
+      <c r="AG5">
+        <v>1.5</v>
+      </c>
+      <c r="AH5" s="17">
+        <v>100</v>
+      </c>
+      <c r="AI5" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ5" s="17">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AK5" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL5" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="AM5" s="17">
+        <v>-0.5</v>
+      </c>
+      <c r="AN5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="17">
         <v>3</v>
       </c>
-      <c r="AD4">
-        <v>25</v>
-      </c>
-      <c r="AE4">
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>700</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <v>3.5</v>
+      </c>
+      <c r="N6">
+        <v>40</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>-8</v>
+      </c>
+      <c r="V6">
+        <v>-1</v>
+      </c>
+      <c r="W6">
+        <v>0.01</v>
+      </c>
+      <c r="X6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="Y6">
+        <v>1E-3</v>
+      </c>
+      <c r="Z6">
+        <v>15</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>1000</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>2</v>
+      </c>
+      <c r="AE6">
+        <v>30</v>
+      </c>
+      <c r="AF6">
+        <v>5</v>
+      </c>
+      <c r="AG6">
+        <v>1.5</v>
+      </c>
+      <c r="AH6" s="17">
+        <v>100</v>
+      </c>
+      <c r="AI6" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ6" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AK6" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL6" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="AM6" s="17">
+        <v>-0.5</v>
+      </c>
+      <c r="AN6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>2.5</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>400</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>3.5</v>
+      </c>
+      <c r="N7">
+        <v>35</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>-8</v>
+      </c>
+      <c r="V7">
+        <v>-1</v>
+      </c>
+      <c r="W7">
+        <v>0.01</v>
+      </c>
+      <c r="X7">
+        <v>1.5E-3</v>
+      </c>
+      <c r="Y7">
+        <v>1E-3</v>
+      </c>
+      <c r="Z7">
+        <v>15</v>
+      </c>
+      <c r="AA7">
+        <v>2</v>
+      </c>
+      <c r="AB7">
+        <v>1000</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>2</v>
+      </c>
+      <c r="AE7">
+        <v>30</v>
+      </c>
+      <c r="AF7">
+        <v>5</v>
+      </c>
+      <c r="AG7">
+        <v>1.5</v>
+      </c>
+      <c r="AH7" s="17">
+        <v>100</v>
+      </c>
+      <c r="AI7" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ7" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AK7" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL7" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="AM7" s="17">
+        <v>-0.5</v>
+      </c>
+      <c r="AN7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="AF4">
-        <v>2.5</v>
-      </c>
-      <c r="AG4" s="17">
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>900</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <v>4.5</v>
+      </c>
+      <c r="N8">
+        <v>50</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>-8</v>
+      </c>
+      <c r="V8">
+        <v>-1</v>
+      </c>
+      <c r="W8">
+        <v>0.01</v>
+      </c>
+      <c r="X8">
+        <v>1.5E-3</v>
+      </c>
+      <c r="Y8">
+        <v>1E-3</v>
+      </c>
+      <c r="Z8">
+        <v>15</v>
+      </c>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1000</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>2</v>
+      </c>
+      <c r="AE8">
+        <v>30</v>
+      </c>
+      <c r="AF8">
+        <v>5</v>
+      </c>
+      <c r="AG8">
+        <v>1.5</v>
+      </c>
+      <c r="AH8" s="17">
         <v>100</v>
       </c>
-      <c r="AH4" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI4" s="17">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="AJ4" s="17">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="AK4" s="17">
+      <c r="AI8" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ8" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AK8" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="AL8" s="17">
         <v>0.05</v>
       </c>
-      <c r="AL4" s="17">
+      <c r="AM8" s="17">
         <v>-0.5</v>
       </c>
-      <c r="AM4" s="17">
+      <c r="AN8" s="17">
         <v>0</v>
       </c>
-      <c r="AN4" s="17">
+      <c r="AO8" s="17">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="N5" s="15"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="N6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update info about input parameters
</commit_message>
<xml_diff>
--- a/data-raw/params_in.xlsx
+++ b/data-raw/params_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620B1AAF-ADF5-154A-BD80-D3B22EAA1AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA70AA-52CC-F846-8AE4-88B684521490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="3600" windowWidth="42000" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7640" yWindow="3600" windowWidth="42000" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -2581,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2593,7 +2593,7 @@
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="188.1640625" customWidth="1"/>
@@ -2684,7 +2684,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
@@ -2716,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>9</v>
@@ -3671,8 +3671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>